<commit_message>
Update Observed data output
</commit_message>
<xml_diff>
--- a/examples/advanced_01/reporting engine input/ObservedData/Chung et al. 2006, po 0.075 mgkg, n=19.xlsx
+++ b/examples/advanced_01/reporting engine input/ObservedData/Chung et al. 2006, po 0.075 mgkg, n=19.xlsx
@@ -19,10 +19,10 @@
     <t>Time [h] [h]</t>
   </si>
   <si>
-    <t>Error [µg/L] [mg/l]</t>
+    <t>C_pls [µg/L] [mg/l]</t>
   </si>
   <si>
-    <t>C_pls [µg/L] [mg/l]</t>
+    <t>Error [µg/L] [mg/l]</t>
   </si>
 </sst>
 </file>
@@ -142,10 +142,10 @@
         <v>0.47213110327720642</v>
       </c>
       <c r="B2" s="15">
+        <v>0.022249998524785042</v>
+      </c>
+      <c r="C2" s="15">
         <v>0.01249999925494194</v>
-      </c>
-      <c r="C2" s="15">
-        <v>0.022249998524785042</v>
       </c>
     </row>
     <row r="3">
@@ -153,10 +153,10 @@
         <v>0.96393436193466187</v>
       </c>
       <c r="B3" s="15">
+        <v>0.018500000238418579</v>
+      </c>
+      <c r="C3" s="15">
         <v>0.0047499998472630978</v>
-      </c>
-      <c r="C3" s="15">
-        <v>0.018500000238418579</v>
       </c>
     </row>
     <row r="4">
@@ -164,10 +164,10 @@
         <v>1.475409984588623</v>
       </c>
       <c r="B4" s="15">
+        <v>0.014249999076128006</v>
+      </c>
+      <c r="C4" s="15">
         <v>0.0044999998062849045</v>
-      </c>
-      <c r="C4" s="15">
-        <v>0.014249999076128006</v>
       </c>
     </row>
     <row r="5">
@@ -175,10 +175,10 @@
         <v>1.9868849515914917</v>
       </c>
       <c r="B5" s="15">
+        <v>0.010999999940395355</v>
+      </c>
+      <c r="C5" s="15">
         <v>0.0047499998472630978</v>
-      </c>
-      <c r="C5" s="15">
-        <v>0.010999999940395355</v>
       </c>
     </row>
     <row r="6">
@@ -186,10 +186,10 @@
         <v>2.9704921245574951</v>
       </c>
       <c r="B6" s="15">
+        <v>0.0059999995864927769</v>
+      </c>
+      <c r="C6" s="15">
         <v>0.0029999997932463884</v>
-      </c>
-      <c r="C6" s="15">
-        <v>0.0059999995864927769</v>
       </c>
     </row>
     <row r="7">
@@ -197,10 +197,10 @@
         <v>3.9737699031829834</v>
       </c>
       <c r="B7" s="15">
+        <v>0.0037499999161809683</v>
+      </c>
+      <c r="C7" s="15">
         <v>0.0017499999376013875</v>
-      </c>
-      <c r="C7" s="15">
-        <v>0.0037499999161809683</v>
       </c>
     </row>
     <row r="8">
@@ -208,10 +208,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="15">
+        <v>0.001999999862164259</v>
+      </c>
+      <c r="C8" s="15">
         <v>0.00099999993108212948</v>
-      </c>
-      <c r="C8" s="15">
-        <v>0.001999999862164259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>